<commit_message>
update data set and data format
</commit_message>
<xml_diff>
--- a/doc/Braess_network_Process_Tutorial.xlsx
+++ b/doc/Braess_network_Process_Tutorial.xlsx
@@ -1,72 +1,120 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\STALite\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99667C7-5A9C-4F5A-B1EF-233BFA8A3AFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="19335" windowHeight="8550"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="In English" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">'In English'!$H$8</definedName>
+    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'In English'!$Q$6:$R$6</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'In English'!$S$7</definedName>
+    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'In English'!$H$8</definedName>
+    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>作者</author>
   </authors>
   <commentList>
-    <comment ref="Q3" authorId="0">
+    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
             <rFont val="SimSun"/>
-            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">
 1. OD demand</t>
         </r>
       </text>
     </comment>
-    <comment ref="Q5" authorId="0">
+    <comment ref="Q5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="SimSun"/>
-            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">2. There are 3 paths from Node 1 to Node 2. </t>
         </r>
       </text>
     </comment>
-    <comment ref="S7" authorId="0">
+    <comment ref="S7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="SimSun"/>
-            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">3. flow on path 3 = demand - flow on paths 1 and 2
 Flow on paths 1 and 2 will be used as "variables" to be changed and optimized.  </t>
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="0">
+    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>12: total system-wide travel time = sum of gaps on different OD pairs</t>
         </r>
@@ -74,7 +122,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 To minimize GAP function
@@ -83,55 +131,52 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q8" authorId="0">
+    <comment ref="Q8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="SimSun"/>
-            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">4. path travel time = sum of link travel time over all links on the path
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="T8" authorId="0">
+    <comment ref="T8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="SimSun"/>
-            <charset val="134"/>
           </rPr>
           <t>5. OD minimum travel time/cost</t>
         </r>
       </text>
     </comment>
-    <comment ref="X8" authorId="0">
+    <comment ref="X8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="SimSun"/>
-            <charset val="134"/>
           </rPr>
           <t>6: traffic assignment UE gap function = path flow *(path cost-OD least cost)
 gap =0 -&gt; user equilibirum</t>
         </r>
       </text>
     </comment>
-    <comment ref="A10" authorId="0">
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">References: 
 </t>
@@ -140,7 +185,7 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve"> Lu, C-C., Mahmassani, H.S. and Zhou, X. (2009) Equivalent Gap Function-Based Reformulation and Solution Algorithm for the Dynamic User 
 Lo, H. K., Chen, A., 2000a. Reformulating the general traffic equilibrium problem via a smooth gap function. Mathematical and Computer Modeling 31(2/3), 179-195.
@@ -149,67 +194,65 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q16" authorId="0">
+    <comment ref="Q16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="SimSun"/>
-            <charset val="134"/>
           </rPr>
           <t>7. the first path of OD 1-&gt;2 passes through link 1-&gt;3.</t>
         </r>
       </text>
     </comment>
-    <comment ref="B37" authorId="0">
+    <comment ref="B37" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>We use beta= 1 to use a linear travel time function (so that the gap function can be converged to 0).</t>
         </r>
       </text>
     </comment>
-    <comment ref="Q37" authorId="0">
+    <comment ref="Q37" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
             <rFont val="SimSun"/>
-            <charset val="134"/>
           </rPr>
           <t xml:space="preserve">8. link flow on the first path = path flow * path-to-link incidence coefficient
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="K38" authorId="0">
+    <comment ref="K38" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>9. total link flow = sum of path flow passing through this link over all paths</t>
         </r>
       </text>
     </comment>
-    <comment ref="M38" authorId="0">
+    <comment ref="M38" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>10: link travel time = BRP function (volume/capacity)
 link cost = link travel time + toll/VOT</t>
@@ -218,21 +261,21 @@
           <rPr>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="Q58" authorId="0">
+    <comment ref="Q58" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="8"/>
             <rFont val="Tahoma"/>
-            <charset val="134"/>
+            <family val="2"/>
           </rPr>
           <t>11. link travel time on this path = corresponding link travel time *0_1_indicator.
 Indicator = 1, if path passes through this link, =0, otherwise</t>
@@ -244,7 +287,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
   <si>
     <t>Author:</t>
   </si>
@@ -421,21 +464,21 @@
   </si>
   <si>
     <t>path travel time</t>
+  </si>
+  <si>
+    <t>]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="0.0"/>
-    <numFmt numFmtId="178" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -444,18 +487,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -463,7 +513,7 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -471,7 +521,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -479,184 +529,38 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <name val="SimSun"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="SimSun"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Tahoma"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
       <name val="Tahoma"/>
-      <charset val="134"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -671,7 +575,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.0999786370433668"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -701,198 +605,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="3" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -1266,342 +984,109 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="36" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1611,65 +1096,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -1686,28 +1135,21 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1723,13 +1165,19 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 38"/>
+        <xdr:cNvPr id="2" name="Picture 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -1766,9 +1214,15 @@
       <xdr:row>25</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1833,9 +1287,15 @@
       <xdr:row>35</xdr:row>
       <xdr:rowOff>114304</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Bent-Up Arrow 11"/>
+        <xdr:cNvPr id="4" name="Bent-Up Arrow 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1887,9 +1347,15 @@
       <xdr:row>43</xdr:row>
       <xdr:rowOff>68099</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Left Arrow 12"/>
+        <xdr:cNvPr id="5" name="Left Arrow 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1941,9 +1407,15 @@
       <xdr:row>48</xdr:row>
       <xdr:rowOff>61966</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="TextBox 5"/>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1993,7 +1465,6 @@
             <a:rPr lang="en-US" sz="1100" b="1"/>
             <a:t>find travel times from the link flows (far left of table)</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2012,9 +1483,15 @@
       <xdr:row>61</xdr:row>
       <xdr:rowOff>109486</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Bent-Up Arrow 14"/>
+        <xdr:cNvPr id="7" name="Bent-Up Arrow 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2066,9 +1543,15 @@
       <xdr:row>52</xdr:row>
       <xdr:rowOff>166634</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="TextBox 7"/>
+        <xdr:cNvPr id="8" name="TextBox 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2141,9 +1624,15 @@
       <xdr:row>60</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Up Arrow 16"/>
+        <xdr:cNvPr id="9" name="Up Arrow 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2195,9 +1684,15 @@
       <xdr:row>58</xdr:row>
       <xdr:rowOff>19051</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
+    <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="TextBox 9"/>
+        <xdr:cNvPr id="10" name="TextBox 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -2254,35 +1749,49 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>22860</xdr:colOff>
           <xdr:row>47</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
+          <xdr:rowOff>30480</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>512051</xdr:colOff>
+          <xdr:colOff>510540</xdr:colOff>
           <xdr:row>51</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
-        <xdr:sp>
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1025" name="Object 1" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="710565" y="9286875"/>
-              <a:ext cx="2435225" cy="733425"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2295,35 +1804,51 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>11</xdr:col>
-          <xdr:colOff>523875</xdr:colOff>
+          <xdr:colOff>525780</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>14</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>30</xdr:row>
-          <xdr:rowOff>161924</xdr:rowOff>
+          <xdr:rowOff>160020</xdr:rowOff>
         </xdr:to>
-        <xdr:sp>
+        <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1026" name="Object 2" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
-              <a:off x="10201275" y="3028950"/>
-              <a:ext cx="3702050" cy="3152140"/>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2331,44 +1856,6 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1280947</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>164224</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>96631</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>22408</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="图片 12"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3750945" y="2373630"/>
-          <a:ext cx="2913380" cy="3668395"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2653,40 +2140,40 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:X61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Y61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.3714285714286" customWidth="1"/>
-    <col min="2" max="2" width="12.5047619047619" customWidth="1"/>
-    <col min="3" max="3" width="16.6285714285714" customWidth="1"/>
-    <col min="4" max="4" width="16.752380952381" customWidth="1"/>
-    <col min="5" max="5" width="11.1238095238095" customWidth="1"/>
-    <col min="6" max="6" width="12.8761904761905" customWidth="1"/>
-    <col min="7" max="7" width="18.247619047619" customWidth="1"/>
-    <col min="8" max="8" width="10.6285714285714" customWidth="1"/>
-    <col min="9" max="9" width="13.752380952381" customWidth="1"/>
-    <col min="10" max="10" width="11.6285714285714" customWidth="1"/>
-    <col min="11" max="11" width="10.6285714285714" customWidth="1"/>
-    <col min="13" max="13" width="22.6285714285714" customWidth="1"/>
-    <col min="14" max="14" width="31.752380952381" customWidth="1"/>
-    <col min="15" max="15" width="22.6285714285714" customWidth="1"/>
-    <col min="16" max="16" width="16.6285714285714" customWidth="1"/>
-    <col min="24" max="24" width="24.247619047619" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.77734375" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" customWidth="1"/>
+    <col min="13" max="13" width="22.6640625" customWidth="1"/>
+    <col min="14" max="14" width="31.77734375" customWidth="1"/>
+    <col min="15" max="15" width="22.6640625" customWidth="1"/>
+    <col min="16" max="16" width="16.6640625" customWidth="1"/>
+    <col min="24" max="24" width="24.21875" customWidth="1"/>
     <col min="25" max="25" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" ht="21" customHeight="1" spans="2:18">
+    <row r="1" spans="1:24" customFormat="1" ht="21" customHeight="1">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2696,241 +2183,247 @@
       <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="N1" s="17" t="s">
         <v>4</v>
       </c>
       <c r="R1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="1" ht="22.5" spans="2:24">
+    <row r="2" spans="1:24" customFormat="1" ht="21">
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="22"/>
-      <c r="M2" s="20">
+      <c r="H2" s="49"/>
+      <c r="I2" s="50"/>
+      <c r="M2" s="16">
         <v>0</v>
       </c>
-      <c r="N2" s="21" t="s">
+      <c r="N2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="23" t="s">
+      <c r="P2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="45" t="s">
+      <c r="Q2" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="46">
+      <c r="R2" s="39">
         <v>0</v>
       </c>
-      <c r="S2" s="45"/>
-      <c r="T2" s="45"/>
-      <c r="U2" s="45"/>
-      <c r="V2" s="45"/>
-      <c r="W2" s="45"/>
-      <c r="X2" s="33"/>
-    </row>
-    <row r="3" customFormat="1" ht="22.5" spans="2:24">
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="26"/>
+    </row>
+    <row r="3" spans="1:24" customFormat="1" ht="21">
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="7" t="s">
+      <c r="G3" s="4"/>
+      <c r="H3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="24"/>
-      <c r="M3" s="20">
+      <c r="I3" s="19"/>
+      <c r="M3" s="16">
         <v>0.65</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="25" t="s">
+      <c r="P3" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="47">
+      <c r="Q3" s="40">
         <v>4000</v>
       </c>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="39"/>
-      <c r="V3" s="39"/>
-      <c r="W3" s="39"/>
-      <c r="X3" s="34"/>
-    </row>
-    <row r="4" customFormat="1" ht="15.75" spans="7:24">
-      <c r="G4" s="8"/>
-      <c r="H4" s="9" t="s">
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="32"/>
+      <c r="U3" s="32"/>
+      <c r="V3" s="32"/>
+      <c r="W3" s="32"/>
+      <c r="X3" s="27"/>
+    </row>
+    <row r="4" spans="1:24" customFormat="1">
+      <c r="G4" s="6"/>
+      <c r="H4" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="26"/>
-      <c r="M4" s="20">
+      <c r="I4" s="52"/>
+      <c r="M4" s="16">
         <v>0.75</v>
       </c>
-      <c r="N4" s="21" t="s">
+      <c r="N4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="39"/>
-      <c r="S4" s="39"/>
-      <c r="T4" s="39"/>
-      <c r="X4" s="34"/>
-    </row>
-    <row r="5" customFormat="1" spans="7:24">
-      <c r="G5" s="10"/>
-      <c r="H5" s="11" t="s">
+      <c r="P4" s="20"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="32"/>
+      <c r="X4" s="27"/>
+    </row>
+    <row r="5" spans="1:24" customFormat="1">
+      <c r="G5" s="7"/>
+      <c r="H5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="27"/>
-      <c r="M5" s="20">
+      <c r="I5" s="21"/>
+      <c r="M5" s="16">
         <v>0.85</v>
       </c>
-      <c r="N5" s="21" t="s">
+      <c r="N5" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="P5" s="28" t="s">
+      <c r="P5" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="45">
+      <c r="Q5" s="38">
         <v>1</v>
       </c>
-      <c r="R5" s="45">
+      <c r="R5" s="38">
         <v>2</v>
       </c>
-      <c r="S5" s="33">
+      <c r="S5" s="26">
         <v>3</v>
       </c>
-      <c r="X5" s="34"/>
-    </row>
-    <row r="6" customFormat="1" ht="15.75" spans="7:24">
-      <c r="G6" s="12"/>
-      <c r="H6" s="13" t="s">
+      <c r="X5" s="27"/>
+    </row>
+    <row r="6" spans="1:24" customFormat="1">
+      <c r="G6" s="9"/>
+      <c r="H6" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="29"/>
-      <c r="M6" s="20">
+      <c r="I6" s="54"/>
+      <c r="M6" s="16">
         <v>0.95</v>
       </c>
-      <c r="N6" s="21" t="s">
+      <c r="N6" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="P6" s="28" t="s">
+      <c r="P6" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="Q6" s="48">
+      <c r="Q6" s="41">
+        <v>400</v>
+      </c>
+      <c r="R6" s="41">
+        <v>3000</v>
+      </c>
+      <c r="S6" s="26">
         <v>0</v>
       </c>
-      <c r="R6" s="48">
+      <c r="T6" s="32"/>
+      <c r="U6" s="55" t="s">
+        <v>23</v>
+      </c>
+      <c r="V6" s="56"/>
+      <c r="W6" s="57"/>
+      <c r="X6" s="27"/>
+    </row>
+    <row r="7" spans="1:24" customFormat="1">
+      <c r="F7" s="11"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="23"/>
+      <c r="M7" s="16">
+        <v>1</v>
+      </c>
+      <c r="N7" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="P7" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q7" s="60" t="s">
+        <v>59</v>
+      </c>
+      <c r="R7" s="42">
         <v>0</v>
       </c>
-      <c r="S6" s="33"/>
-      <c r="T6" s="39"/>
-      <c r="U6" s="49" t="s">
-        <v>23</v>
-      </c>
-      <c r="V6" s="50"/>
-      <c r="W6" s="51"/>
-      <c r="X6" s="34"/>
-    </row>
-    <row r="7" customFormat="1" ht="15.75" spans="6:24">
-      <c r="F7" s="14"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="29"/>
-      <c r="M7" s="20">
+      <c r="S7" s="43">
+        <f>Q3-Q6-R6</f>
+        <v>600</v>
+      </c>
+      <c r="T7" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="U7" s="20">
         <v>1</v>
       </c>
-      <c r="N7" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="P7" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q7" s="52"/>
-      <c r="R7" s="52"/>
-      <c r="S7" s="53">
-        <f>Q3-Q6-R6</f>
-        <v>4000</v>
-      </c>
-      <c r="T7" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="U7" s="25">
-        <v>1</v>
-      </c>
-      <c r="V7" s="39">
+      <c r="V7" s="32">
         <v>2</v>
       </c>
-      <c r="W7" s="34">
+      <c r="W7" s="27">
         <v>3</v>
       </c>
-      <c r="X7" s="28" t="s">
+      <c r="X7" s="22" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" customFormat="1" ht="15.75" spans="6:24">
-      <c r="F8" s="14"/>
-      <c r="G8" s="16" t="s">
+    <row r="8" spans="1:24" customFormat="1">
+      <c r="F8" s="11"/>
+      <c r="G8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="58">
         <f>X8</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="31"/>
-      <c r="P8" s="32" t="s">
+        <v>108562.59993738537</v>
+      </c>
+      <c r="I8" s="59"/>
+      <c r="P8" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="Q8" s="54">
+      <c r="Q8" s="44">
         <f>SUM(Q57:Q61)</f>
-        <v>85.01</v>
-      </c>
-      <c r="R8" s="54">
+        <v>55.01</v>
+      </c>
+      <c r="R8" s="44">
         <f>SUM(R57:R61)</f>
-        <v>85.01</v>
-      </c>
-      <c r="S8" s="55">
+        <v>81.009999999999991</v>
+      </c>
+      <c r="S8" s="45">
         <f>SUM(S57:S61)</f>
-        <v>80.0210363774122</v>
-      </c>
-      <c r="T8" s="36">
+        <v>46.021000018416061</v>
+      </c>
+      <c r="T8" s="29">
         <f>MIN(Q8:S8)</f>
-        <v>80.0210363774122</v>
-      </c>
-      <c r="U8" s="36">
+        <v>46.021000018416061</v>
+      </c>
+      <c r="U8" s="29">
         <f>(Q8-$T$8)*Q6</f>
-        <v>0</v>
-      </c>
-      <c r="V8" s="56">
+        <v>3595.5999926335749</v>
+      </c>
+      <c r="V8" s="46">
         <f t="shared" ref="V8" si="0">(R8-$T$8)*R6</f>
-        <v>0</v>
-      </c>
-      <c r="W8" s="37">
+        <v>104966.99994475179</v>
+      </c>
+      <c r="W8" s="30">
         <f>(S8-$T$8)*S7</f>
         <v>0</v>
       </c>
-      <c r="X8" s="57">
+      <c r="X8" s="47">
         <f>SUM(U8:W8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" customFormat="1" spans="1:1">
-      <c r="A10" s="18" t="s">
+        <v>108562.59993738537</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" customFormat="1">
+      <c r="A10" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" customFormat="1" spans="17:19">
+    <row r="14" spans="1:24" customFormat="1">
       <c r="Q14" t="s">
         <v>31</v>
       </c>
@@ -2941,157 +2434,157 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" customFormat="1" spans="9:17">
-      <c r="I15" s="23" t="s">
+    <row r="15" spans="1:24" customFormat="1">
+      <c r="I15" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="J15" s="33" t="s">
+      <c r="J15" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="Q15" s="18" t="s">
+      <c r="Q15" s="14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" customFormat="1" spans="9:19">
-      <c r="I16" s="25">
+    <row r="16" spans="1:24" customFormat="1">
+      <c r="I16" s="20">
         <v>1</v>
       </c>
-      <c r="J16" s="34">
+      <c r="J16" s="27">
         <v>3</v>
       </c>
       <c r="P16" t="s">
         <v>37</v>
       </c>
-      <c r="Q16" s="23">
+      <c r="Q16" s="18">
         <v>1</v>
       </c>
-      <c r="R16" s="45"/>
-      <c r="S16" s="33">
+      <c r="R16" s="38"/>
+      <c r="S16" s="26">
         <v>1</v>
       </c>
     </row>
-    <row r="17" customFormat="1" spans="9:19">
-      <c r="I17" s="25">
+    <row r="17" spans="9:19" customFormat="1">
+      <c r="I17" s="20">
         <v>1</v>
       </c>
-      <c r="J17" s="34">
+      <c r="J17" s="27">
         <v>4</v>
       </c>
       <c r="P17" t="s">
         <v>38</v>
       </c>
-      <c r="Q17" s="25"/>
-      <c r="R17" s="39">
+      <c r="Q17" s="20"/>
+      <c r="R17" s="32">
         <v>1</v>
       </c>
-      <c r="S17" s="34"/>
-    </row>
-    <row r="18" customFormat="1" spans="9:19">
-      <c r="I18" s="25">
+      <c r="S17" s="27"/>
+    </row>
+    <row r="18" spans="9:19" customFormat="1">
+      <c r="I18" s="20">
         <v>3</v>
       </c>
-      <c r="J18" s="34">
+      <c r="J18" s="27">
         <v>2</v>
       </c>
-      <c r="M18" s="35">
+      <c r="M18" s="28">
         <f>$K$37</f>
-        <v>4000</v>
-      </c>
-      <c r="N18" s="35">
+        <v>1000</v>
+      </c>
+      <c r="N18" s="28">
         <f>$K$39</f>
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="P18" t="s">
         <v>39</v>
       </c>
-      <c r="Q18" s="25">
+      <c r="Q18" s="20">
         <v>1</v>
       </c>
-      <c r="R18" s="39"/>
-      <c r="S18" s="34"/>
-    </row>
-    <row r="19" customFormat="1" spans="9:19">
-      <c r="I19" s="25">
+      <c r="R18" s="32"/>
+      <c r="S18" s="27"/>
+    </row>
+    <row r="19" spans="9:19" customFormat="1">
+      <c r="I19" s="20">
         <v>3</v>
       </c>
-      <c r="J19" s="34">
+      <c r="J19" s="27">
         <v>4</v>
       </c>
       <c r="P19" t="s">
         <v>40</v>
       </c>
-      <c r="Q19" s="25"/>
-      <c r="R19" s="39"/>
-      <c r="S19" s="34">
+      <c r="Q19" s="20"/>
+      <c r="R19" s="32"/>
+      <c r="S19" s="27">
         <v>1</v>
       </c>
     </row>
-    <row r="20" customFormat="1" spans="9:19">
-      <c r="I20" s="36">
+    <row r="20" spans="9:19" customFormat="1">
+      <c r="I20" s="29">
         <v>4</v>
       </c>
-      <c r="J20" s="37">
+      <c r="J20" s="30">
         <v>2</v>
       </c>
       <c r="P20" t="s">
         <v>41</v>
       </c>
-      <c r="Q20" s="36"/>
-      <c r="R20" s="56">
+      <c r="Q20" s="29"/>
+      <c r="R20" s="46">
         <v>1</v>
       </c>
-      <c r="S20" s="37">
+      <c r="S20" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="23" customFormat="1" spans="14:14">
-      <c r="N23" s="38">
+    <row r="23" spans="9:19" customFormat="1">
+      <c r="N23" s="31">
         <f>$K$40</f>
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="25" customFormat="1" spans="15:15">
-      <c r="O25" s="39"/>
-    </row>
-    <row r="28" customFormat="1" spans="14:15">
-      <c r="N28" s="35"/>
-      <c r="O28" s="39"/>
-    </row>
-    <row r="29" customFormat="1" spans="13:14">
-      <c r="M29" s="35">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="25" spans="9:19" customFormat="1">
+      <c r="O25" s="32"/>
+    </row>
+    <row r="28" spans="9:19" customFormat="1">
+      <c r="N28" s="28"/>
+      <c r="O28" s="32"/>
+    </row>
+    <row r="29" spans="9:19" customFormat="1">
+      <c r="M29" s="28">
         <f>$K$38</f>
-        <v>0</v>
-      </c>
-      <c r="N29" s="35">
+        <v>3000</v>
+      </c>
+      <c r="N29" s="28">
         <f>$K$41</f>
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="33" customFormat="1" spans="12:13">
-      <c r="L33" s="19" t="s">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" customFormat="1">
+      <c r="L33" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="M33" s="19">
+      <c r="M33" s="15">
         <v>10</v>
       </c>
     </row>
-    <row r="36" customFormat="1" spans="1:17">
-      <c r="A36" s="19" t="s">
+    <row r="36" spans="1:19" customFormat="1">
+      <c r="A36" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="19" t="s">
+      <c r="C36" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="D36" s="19" t="s">
+      <c r="D36" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="E36" s="19" t="s">
+      <c r="E36" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F36" s="19" t="s">
+      <c r="F36" s="15" t="s">
         <v>48</v>
       </c>
       <c r="G36" t="s">
@@ -3103,7 +2596,7 @@
       <c r="I36" t="s">
         <v>35</v>
       </c>
-      <c r="J36" s="40" t="s">
+      <c r="J36" s="33" t="s">
         <v>50</v>
       </c>
       <c r="K36" t="s">
@@ -3125,7 +2618,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" customFormat="1" spans="1:19">
+    <row r="37" spans="1:19" customFormat="1">
       <c r="A37" s="1">
         <v>100</v>
       </c>
@@ -3153,43 +2646,43 @@
       <c r="I37" s="1">
         <v>3</v>
       </c>
-      <c r="J37" s="41">
+      <c r="J37" s="34">
         <f>C37/E37*60</f>
         <v>0.01</v>
       </c>
-      <c r="K37" s="42">
+      <c r="K37" s="35">
         <f>SUM(Q37:S37)</f>
-        <v>4000</v>
+        <v>1000</v>
       </c>
       <c r="L37" s="1">
         <v>0</v>
       </c>
-      <c r="M37" s="43">
+      <c r="M37" s="36">
         <f>J37*(1+A37*POWER(K37/(D37*F37),B37))+L37/$M$33</f>
-        <v>40.01</v>
-      </c>
-      <c r="N37" s="44">
+        <v>10.01</v>
+      </c>
+      <c r="N37" s="37">
         <f t="shared" ref="N37:N41" si="1">K37/(F37*D37)</f>
-        <v>40</v>
-      </c>
-      <c r="O37" s="43" t="str">
+        <v>10</v>
+      </c>
+      <c r="O37" s="36" t="str">
         <f>VLOOKUP(N37,$M$2:$N$7,2,TRUE)</f>
         <v>F</v>
       </c>
-      <c r="Q37" s="23">
+      <c r="Q37" s="18">
         <f t="shared" ref="Q37:R41" si="2">Q$6*Q16</f>
-        <v>0</v>
-      </c>
-      <c r="R37" s="45">
+        <v>400</v>
+      </c>
+      <c r="R37" s="38">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S37" s="33">
+      <c r="S37" s="26">
         <f t="shared" ref="S37:S41" si="3">S$7*S16</f>
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="38" customFormat="1" spans="1:19">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" customFormat="1">
       <c r="A38" s="1">
         <v>0</v>
       </c>
@@ -3217,43 +2710,43 @@
       <c r="I38" s="1">
         <v>4</v>
       </c>
-      <c r="J38" s="41">
+      <c r="J38" s="34">
         <f t="shared" ref="J38:J41" si="4">C38/E38*60</f>
         <v>45</v>
       </c>
-      <c r="K38" s="42">
+      <c r="K38" s="35">
         <f>SUM(Q38:S38)</f>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="L38" s="1">
         <v>0</v>
       </c>
-      <c r="M38" s="43">
+      <c r="M38" s="36">
         <f t="shared" ref="M38:M41" si="5">J38*(1+A38*POWER(K38/(D38*F38),B38))+L38/$M$33</f>
         <v>45</v>
       </c>
-      <c r="N38" s="44">
+      <c r="N38" s="37">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O38" s="43" t="str">
+        <v>0.52631578947368418</v>
+      </c>
+      <c r="O38" s="36" t="str">
         <f t="shared" ref="O38:O41" si="6">VLOOKUP(N38,$M$2:$N$7,2,TRUE)</f>
         <v>A</v>
       </c>
-      <c r="Q38" s="25">
+      <c r="Q38" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R38" s="39">
+      <c r="R38" s="32">
         <f>R$6*R17</f>
-        <v>0</v>
-      </c>
-      <c r="S38" s="34">
+        <v>3000</v>
+      </c>
+      <c r="S38" s="27">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="39" customFormat="1" spans="1:19">
+    <row r="39" spans="1:19" customFormat="1">
       <c r="A39" s="1">
         <v>0</v>
       </c>
@@ -3281,253 +2774,253 @@
       <c r="I39" s="1">
         <v>2</v>
       </c>
-      <c r="J39" s="41">
+      <c r="J39" s="34">
         <f t="shared" si="4"/>
         <v>45</v>
       </c>
-      <c r="K39" s="42">
+      <c r="K39" s="35">
         <f>SUM(Q39:S39)</f>
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="L39" s="1">
         <v>0</v>
       </c>
-      <c r="M39" s="43">
+      <c r="M39" s="36">
         <f t="shared" si="5"/>
         <v>45</v>
       </c>
-      <c r="N39" s="44">
+      <c r="N39" s="37">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O39" s="43" t="str">
+        <v>7.0175438596491224E-2</v>
+      </c>
+      <c r="O39" s="36" t="str">
         <f t="shared" si="6"/>
         <v>A</v>
       </c>
-      <c r="Q39" s="25">
+      <c r="Q39" s="20">
+        <f t="shared" si="2"/>
+        <v>400</v>
+      </c>
+      <c r="R39" s="32">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R39" s="39">
+      <c r="S39" s="27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" customFormat="1">
+      <c r="A40" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="B40" s="1">
+        <v>4</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="D40" s="1">
+        <v>3</v>
+      </c>
+      <c r="E40" s="1">
+        <v>65</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1900</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40" s="1">
+        <v>3</v>
+      </c>
+      <c r="I40" s="1">
+        <v>4</v>
+      </c>
+      <c r="J40" s="34">
+        <v>1E-3</v>
+      </c>
+      <c r="K40" s="35">
+        <f>SUM(Q40:S40)</f>
+        <v>600</v>
+      </c>
+      <c r="L40" s="1">
+        <v>0</v>
+      </c>
+      <c r="M40" s="36">
+        <f t="shared" si="5"/>
+        <v>1.0000184160649473E-3</v>
+      </c>
+      <c r="N40" s="37">
+        <f t="shared" si="1"/>
+        <v>0.10526315789473684</v>
+      </c>
+      <c r="O40" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v>A</v>
+      </c>
+      <c r="Q40" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S39" s="34">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" customFormat="1" spans="1:19">
-      <c r="A40" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="B40" s="1">
-        <v>4</v>
-      </c>
-      <c r="C40" s="1">
-        <v>0.001</v>
-      </c>
-      <c r="D40" s="1">
-        <v>3</v>
-      </c>
-      <c r="E40" s="1">
-        <v>65</v>
-      </c>
-      <c r="F40" s="1">
-        <v>1900</v>
-      </c>
-      <c r="G40">
-        <v>1</v>
-      </c>
-      <c r="H40" s="1">
-        <v>3</v>
-      </c>
-      <c r="I40" s="1">
-        <v>4</v>
-      </c>
-      <c r="J40" s="41">
-        <v>0.001</v>
-      </c>
-      <c r="K40" s="42">
-        <f>SUM(Q40:S40)</f>
-        <v>4000</v>
-      </c>
-      <c r="L40" s="1">
-        <v>0</v>
-      </c>
-      <c r="M40" s="43">
-        <f t="shared" si="5"/>
-        <v>0.00103637741224162</v>
-      </c>
-      <c r="N40" s="44">
-        <f t="shared" si="1"/>
-        <v>0.701754385964912</v>
-      </c>
-      <c r="O40" s="43" t="str">
-        <f t="shared" si="6"/>
-        <v>B</v>
-      </c>
-      <c r="Q40" s="25">
+      <c r="R40" s="32">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R40" s="39">
+      <c r="S40" s="27">
+        <f t="shared" si="3"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" customFormat="1">
+      <c r="A41" s="1">
+        <v>100</v>
+      </c>
+      <c r="B41" s="1">
+        <v>1</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1</v>
+      </c>
+      <c r="E41" s="1">
+        <v>60</v>
+      </c>
+      <c r="F41" s="1">
+        <v>100</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41" s="1">
+        <v>4</v>
+      </c>
+      <c r="I41" s="1">
+        <v>2</v>
+      </c>
+      <c r="J41" s="34">
+        <f t="shared" si="4"/>
+        <v>0.01</v>
+      </c>
+      <c r="K41" s="35">
+        <f>SUM(Q41:S41)</f>
+        <v>3600</v>
+      </c>
+      <c r="L41" s="1">
+        <v>0</v>
+      </c>
+      <c r="M41" s="36">
+        <f t="shared" si="5"/>
+        <v>36.01</v>
+      </c>
+      <c r="N41" s="37">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="O41" s="36" t="str">
+        <f t="shared" si="6"/>
+        <v>F</v>
+      </c>
+      <c r="Q41" s="29">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S40" s="34">
+      <c r="R41" s="46">
+        <f t="shared" si="2"/>
+        <v>3000</v>
+      </c>
+      <c r="S41" s="30">
         <f t="shared" si="3"/>
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="41" customFormat="1" spans="1:19">
-      <c r="A41" s="1">
-        <v>100</v>
-      </c>
-      <c r="B41" s="1">
-        <v>1</v>
-      </c>
-      <c r="C41" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="D41" s="1">
-        <v>1</v>
-      </c>
-      <c r="E41" s="1">
-        <v>60</v>
-      </c>
-      <c r="F41" s="1">
-        <v>100</v>
-      </c>
-      <c r="G41">
-        <v>1</v>
-      </c>
-      <c r="H41" s="1">
-        <v>4</v>
-      </c>
-      <c r="I41" s="1">
-        <v>2</v>
-      </c>
-      <c r="J41" s="41">
-        <f t="shared" si="4"/>
-        <v>0.01</v>
-      </c>
-      <c r="K41" s="42">
-        <f>SUM(Q41:S41)</f>
-        <v>4000</v>
-      </c>
-      <c r="L41" s="1">
-        <v>0</v>
-      </c>
-      <c r="M41" s="43">
-        <f t="shared" si="5"/>
-        <v>40.01</v>
-      </c>
-      <c r="N41" s="44">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="O41" s="43" t="str">
-        <f t="shared" si="6"/>
-        <v>F</v>
-      </c>
-      <c r="Q41" s="36">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R41" s="56">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="S41" s="37">
-        <f t="shared" si="3"/>
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="42" customFormat="1" spans="12:12">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" customFormat="1">
       <c r="L42" s="1"/>
     </row>
-    <row r="43" customFormat="1" spans="12:12">
+    <row r="43" spans="1:19" customFormat="1">
       <c r="L43" s="1"/>
     </row>
-    <row r="46" customFormat="1" spans="2:2">
-      <c r="B46" s="18" t="s">
+    <row r="46" spans="1:19" customFormat="1">
+      <c r="B46" s="14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="56" customFormat="1" spans="17:17">
+    <row r="56" spans="17:19" customFormat="1">
       <c r="Q56" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="57" customFormat="1" spans="17:19">
-      <c r="Q57" s="23">
+    <row r="57" spans="17:19" customFormat="1">
+      <c r="Q57" s="18">
         <f>$M37*Q16</f>
-        <v>40.01</v>
-      </c>
-      <c r="R57" s="45">
+        <v>10.01</v>
+      </c>
+      <c r="R57" s="38">
         <f>$M37*R16</f>
         <v>0</v>
       </c>
-      <c r="S57" s="33">
+      <c r="S57" s="26">
         <f>$M37*S16</f>
-        <v>40.01</v>
-      </c>
-    </row>
-    <row r="58" customFormat="1" spans="17:19">
-      <c r="Q58" s="25">
+        <v>10.01</v>
+      </c>
+    </row>
+    <row r="58" spans="17:19" customFormat="1">
+      <c r="Q58" s="20">
         <f t="shared" ref="Q58:S61" si="7">$M38*Q17</f>
         <v>0</v>
       </c>
-      <c r="R58" s="39">
+      <c r="R58" s="32">
         <f t="shared" si="7"/>
         <v>45</v>
       </c>
-      <c r="S58" s="34">
+      <c r="S58" s="27">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="59" customFormat="1" spans="17:19">
-      <c r="Q59" s="25">
+    <row r="59" spans="17:19" customFormat="1">
+      <c r="Q59" s="20">
         <f t="shared" si="7"/>
         <v>45</v>
       </c>
-      <c r="R59" s="39">
+      <c r="R59" s="32">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="S59" s="34">
+      <c r="S59" s="27">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="60" customFormat="1" spans="17:19">
-      <c r="Q60" s="25">
+    <row r="60" spans="17:19" customFormat="1">
+      <c r="Q60" s="20">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="R60" s="39">
+      <c r="R60" s="32">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="S60" s="34">
+      <c r="S60" s="27">
         <f t="shared" si="7"/>
-        <v>0.00103637741224162</v>
-      </c>
-    </row>
-    <row r="61" customFormat="1" spans="17:19">
-      <c r="Q61" s="36">
+        <v>1.0000184160649473E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="17:19" customFormat="1">
+      <c r="Q61" s="29">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="R61" s="56">
+      <c r="R61" s="46">
         <f t="shared" si="7"/>
-        <v>40.01</v>
-      </c>
-      <c r="S61" s="37">
+        <v>36.01</v>
+      </c>
+      <c r="S61" s="30">
         <f t="shared" si="7"/>
-        <v>40.01</v>
+        <v>36.01</v>
       </c>
     </row>
   </sheetData>
@@ -3545,11 +3038,6 @@
         <cfvo type="max"/>
         <color rgb="FFFF555A"/>
       </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{e3a0b399-2f0d-4b1e-b127-9986d0b055d9}</x14:id>
-        </ext>
-      </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O37:O41">
@@ -3561,10 +3049,10 @@
         <cfvo type="percent" val="75"/>
       </iconSet>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
       <formula>"C"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">
@@ -3579,24 +3067,23 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <oleObjects>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject shapeId="1025" progId="Equation.3" r:id="rId4">
-          <objectPr defaultSize="0" r:id="rId5">
+        <oleObject progId="Equation.3" shapeId="1025" r:id="rId3">
+          <objectPr defaultSize="0" altText="" r:id="rId4">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:colOff>22860</xdr:colOff>
                 <xdr:row>47</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:rowOff>30480</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>511810</xdr:colOff>
+                <xdr:colOff>510540</xdr:colOff>
                 <xdr:row>51</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -3605,50 +3092,34 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject shapeId="1025" progId="Equation.3" r:id="rId4"/>
+        <oleObject progId="Equation.3" shapeId="1025" r:id="rId3"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject shapeId="1026" progId="Visio.Drawing.11" r:id="rId6">
-          <objectPr defaultSize="0" r:id="rId7">
+        <oleObject progId="Visio.Drawing.11" shapeId="1026" r:id="rId5">
+          <objectPr defaultSize="0" altText="" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>11</xdr:col>
-                <xdr:colOff>523875</xdr:colOff>
+                <xdr:colOff>525780</xdr:colOff>
                 <xdr:row>14</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
+                <xdr:rowOff>60960</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>14</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
                 <xdr:row>30</xdr:row>
-                <xdr:rowOff>161290</xdr:rowOff>
+                <xdr:rowOff>160020</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject shapeId="1026" progId="Visio.Drawing.11" r:id="rId6"/>
+        <oleObject progId="Visio.Drawing.11" shapeId="1026" r:id="rId5"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </oleObjects>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{e3a0b399-2f0d-4b1e-b127-9986d0b055d9}">
-            <x14:dataBar minLength="10" maxLength="90" negativeBarColorSameAsPositive="1" axisPosition="none">
-              <x14:cfvo type="min"/>
-              <x14:cfvo type="max"/>
-              <x14:axisColor indexed="65"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>N37:N41</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>